<commit_message>
predictive table epsilon update
</commit_message>
<xml_diff>
--- a/ex2/PredictiveTable.xlsx
+++ b/ex2/PredictiveTable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1lab500\Source\Repos\CompilationHIT\ex2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="107">
   <si>
     <t>TOKEN</t>
   </si>
@@ -178,9 +178,6 @@
     <t>;</t>
   </si>
   <si>
-    <t xml:space="preserve"> ; VAR_DEFINITIONS</t>
-  </si>
-  <si>
     <t xml:space="preserve">VARIABLE# </t>
   </si>
   <si>
@@ -338,6 +335,12 @@
   </si>
   <si>
     <t>,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ; VAR_DEFINITIONS | epsilon</t>
+  </si>
+  <si>
+    <t>epsilon</t>
   </si>
 </sst>
 </file>
@@ -348,21 +351,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -370,7 +373,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -378,7 +381,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -386,35 +389,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -422,7 +425,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -430,14 +433,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -445,14 +448,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -460,7 +463,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -468,19 +471,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -681,6 +684,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1069,7 +1078,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1140,6 +1149,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1466,38 +1478,38 @@
   <dimension ref="A1:X22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X15" sqref="X15"/>
+      <selection pane="bottomRight" activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="37" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="48" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="33.25" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1574,7 +1586,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>24</v>
       </c>
@@ -1604,7 +1616,7 @@
       <c r="W2" s="8"/>
       <c r="X2" s="9"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>26</v>
       </c>
@@ -1623,7 +1635,9 @@
       <c r="N3" s="12"/>
       <c r="O3" s="12"/>
       <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
+      <c r="Q3" s="12" t="s">
+        <v>106</v>
+      </c>
       <c r="R3" s="12"/>
       <c r="S3" s="12"/>
       <c r="T3" s="12"/>
@@ -1632,7 +1646,7 @@
       <c r="W3" s="12"/>
       <c r="X3" s="13"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>27</v>
       </c>
@@ -1676,7 +1690,7 @@
       <c r="W4" s="12"/>
       <c r="X4" s="13"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>36</v>
       </c>
@@ -1720,7 +1734,7 @@
       <c r="W5" s="12"/>
       <c r="X5" s="13"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>38</v>
       </c>
@@ -1756,7 +1770,7 @@
       <c r="W6" s="12"/>
       <c r="X6" s="13"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>40</v>
       </c>
@@ -1790,7 +1804,7 @@
       <c r="W7" s="12"/>
       <c r="X7" s="13"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>44</v>
       </c>
@@ -1802,7 +1816,9 @@
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
+      <c r="J8" s="12" t="s">
+        <v>106</v>
+      </c>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
@@ -1820,7 +1836,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>46</v>
       </c>
@@ -1850,7 +1866,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>48</v>
       </c>
@@ -1880,9 +1896,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="12"/>
@@ -1894,7 +1910,9 @@
         <v>50</v>
       </c>
       <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
+      <c r="J11" s="12" t="s">
+        <v>106</v>
+      </c>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
@@ -1910,21 +1928,25 @@
       <c r="W11" s="12"/>
       <c r="X11" s="13"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="12"/>
-      <c r="D12" s="12" t="s">
-        <v>52</v>
+      <c r="D12" s="36" t="s">
+        <v>105</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
+      <c r="H12" s="12" t="s">
+        <v>106</v>
+      </c>
       <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
+      <c r="J12" s="12" t="s">
+        <v>106</v>
+      </c>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
@@ -1933,18 +1955,20 @@
       <c r="P12" s="12"/>
       <c r="Q12" s="12"/>
       <c r="R12" s="12"/>
-      <c r="S12" s="12"/>
+      <c r="S12" s="12" t="s">
+        <v>106</v>
+      </c>
       <c r="T12" s="12"/>
       <c r="U12" s="12"/>
       <c r="V12" s="12"/>
       <c r="W12" s="12"/>
       <c r="X12" s="35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>54</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
@@ -1965,16 +1989,16 @@
       <c r="R13" s="12"/>
       <c r="S13" s="12"/>
       <c r="T13" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U13" s="12"/>
       <c r="V13" s="12"/>
       <c r="W13" s="12"/>
       <c r="X13" s="13"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
@@ -1982,27 +2006,35 @@
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
+      <c r="H14" s="12" t="s">
+        <v>106</v>
+      </c>
       <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
+      <c r="J14" s="12" t="s">
+        <v>106</v>
+      </c>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
+      <c r="O14" s="12" t="s">
+        <v>106</v>
+      </c>
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
       <c r="R14" s="12"/>
       <c r="S14" s="12"/>
       <c r="T14" s="12"/>
       <c r="U14" s="12"/>
-      <c r="V14" s="12"/>
+      <c r="V14" s="12" t="s">
+        <v>106</v>
+      </c>
       <c r="W14" s="12"/>
       <c r="X14" s="13"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
@@ -2013,7 +2045,7 @@
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
@@ -2025,18 +2057,18 @@
       <c r="R15" s="12"/>
       <c r="S15" s="12"/>
       <c r="T15" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U15" s="12"/>
       <c r="V15" s="12"/>
       <c r="W15" s="12"/>
       <c r="X15" s="35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
@@ -2062,9 +2094,9 @@
       <c r="W16" s="12"/>
       <c r="X16" s="13"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="12"/>
@@ -2087,20 +2119,20 @@
         <v>42</v>
       </c>
       <c r="R17" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S17" s="12"/>
       <c r="T17" s="12"/>
       <c r="U17" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V17" s="12"/>
       <c r="W17" s="12"/>
       <c r="X17" s="13"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="12"/>
@@ -2117,7 +2149,9 @@
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
-      <c r="Q18" s="12"/>
+      <c r="Q18" s="12" t="s">
+        <v>106</v>
+      </c>
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
       <c r="T18" s="12"/>
@@ -2126,9 +2160,9 @@
       <c r="W18" s="12"/>
       <c r="X18" s="13"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="12"/>
@@ -2136,11 +2170,11 @@
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
       <c r="G19" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
@@ -2155,24 +2189,24 @@
         <v>42</v>
       </c>
       <c r="R19" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="S19" s="12" t="s">
         <v>68</v>
-      </c>
-      <c r="S19" s="12" t="s">
-        <v>69</v>
       </c>
       <c r="T19" s="12"/>
       <c r="U19" s="12"/>
       <c r="V19" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="W19" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="W19" s="12" t="s">
+      <c r="X19" s="13"/>
+    </row>
+    <row r="20" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="X19" s="13"/>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>72</v>
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="12"/>
@@ -2192,19 +2226,19 @@
       <c r="Q20" s="12"/>
       <c r="R20" s="12"/>
       <c r="S20" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T20" s="12"/>
       <c r="U20" s="12"/>
       <c r="V20" s="12"/>
       <c r="W20" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="X20" s="13"/>
+    </row>
+    <row r="21" spans="1:24" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>73</v>
-      </c>
-      <c r="X20" s="13"/>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>74</v>
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="12"/>
@@ -2224,19 +2258,19 @@
       <c r="Q21" s="12"/>
       <c r="R21" s="12"/>
       <c r="S21" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T21" s="12"/>
       <c r="U21" s="12"/>
       <c r="V21" s="12"/>
       <c r="W21" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X21" s="13"/>
     </row>
     <row r="22" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
@@ -2248,7 +2282,9 @@
       <c r="I22" s="16"/>
       <c r="J22" s="16"/>
       <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
+      <c r="L22" s="16" t="s">
+        <v>106</v>
+      </c>
       <c r="M22" s="16"/>
       <c r="N22" s="16"/>
       <c r="O22" s="16"/>
@@ -2275,29 +2311,29 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="C1" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="D1" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="33" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
@@ -2305,13 +2341,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>2</v>
       </c>
@@ -2319,13 +2355,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>3</v>
       </c>
@@ -2333,13 +2369,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>4</v>
       </c>
@@ -2347,13 +2383,13 @@
         <v>0</v>
       </c>
       <c r="C5" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>5</v>
       </c>
@@ -2361,13 +2397,13 @@
         <v>0</v>
       </c>
       <c r="C6" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>6</v>
       </c>
@@ -2375,13 +2411,13 @@
         <v>0</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>7</v>
       </c>
@@ -2389,13 +2425,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>8</v>
       </c>
@@ -2403,13 +2439,13 @@
         <v>0</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>9</v>
       </c>
@@ -2417,13 +2453,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="23" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>10</v>
       </c>
@@ -2431,13 +2467,13 @@
         <v>0</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>11</v>
       </c>
@@ -2445,13 +2481,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>12</v>
       </c>
@@ -2459,13 +2495,13 @@
         <v>0</v>
       </c>
       <c r="C13" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="23" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
         <v>13</v>
       </c>
@@ -2473,13 +2509,13 @@
         <v>0</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>14</v>
       </c>
@@ -2487,13 +2523,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
         <v>15</v>
       </c>
@@ -2501,13 +2537,13 @@
         <v>0</v>
       </c>
       <c r="C16" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="23" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>16</v>
       </c>
@@ -2515,13 +2551,13 @@
         <v>1</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
         <v>17</v>
       </c>
@@ -2529,13 +2565,13 @@
         <v>0</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
         <v>18</v>
       </c>
@@ -2543,13 +2579,13 @@
         <v>1</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
         <v>19</v>
       </c>
@@ -2557,13 +2593,13 @@
         <v>0</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
         <v>20</v>
       </c>
@@ -2571,13 +2607,13 @@
         <v>0</v>
       </c>
       <c r="C21" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="D21" s="23" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
         <v>21</v>
       </c>
@@ -2585,13 +2621,13 @@
         <v>1</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>22</v>
       </c>
@@ -2599,10 +2635,10 @@
         <v>0</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2613,10 +2649,10 @@
         <v>1</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
no massege on finish
</commit_message>
<xml_diff>
--- a/ex2/PredictiveTable.xlsx
+++ b/ex2/PredictiveTable.xlsx
@@ -689,7 +689,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1475,10 +1475,10 @@
   <dimension ref="A1:X22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T8" sqref="T8"/>
+      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>